<commit_message>
Direct Mapped Cache in Report
</commit_message>
<xml_diff>
--- a/Lab6/doc/direct.xlsx
+++ b/Lab6/doc/direct.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wei\Desktop\git\CompOrgTeam\Lab6\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wei\Desktop\git\CompOrgTeam\Lab6\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{CFB75F7B-DDE4-4206-87EF-4592F4F3705D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B1FCEA-6C4A-4DC1-9FAD-89A94BD1781B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11784" windowHeight="5580" xr2:uid="{16BA1ED8-CE1F-49DE-B399-B70958820241}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11790" windowHeight="5580" xr2:uid="{16BA1ED8-CE1F-49DE-B399-B70958820241}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +91,14 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,19 +116,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -150,6 +183,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>Direct Mapped Cache - Instruction cache</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -190,7 +249,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$3</c:f>
+              <c:f>工作表1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -223,9 +282,67 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$2:$F$2</c:f>
+              <c:f>工作表1!$C$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -248,24 +365,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$3:$F$3</c:f>
+              <c:f>工作表1!$C$4:$G$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.17</c:v>
+                  <c:v>2.1700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27</c:v>
+                  <c:v>2.7000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,7 +399,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$4</c:f>
+              <c:f>工作表1!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -315,9 +432,67 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$2:$F$2</c:f>
+              <c:f>工作表1!$C$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -340,24 +515,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$4:$F$4</c:f>
+              <c:f>工作表1!$C$5:$G$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.17</c:v>
+                  <c:v>2.1700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27</c:v>
+                  <c:v>2.7000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,7 +549,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$5</c:f>
+              <c:f>工作表1!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -407,9 +582,67 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$2:$F$2</c:f>
+              <c:f>工作表1!$C$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -432,24 +665,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$5:$F$5</c:f>
+              <c:f>工作表1!$C$6:$G$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.17</c:v>
+                  <c:v>2.1700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27</c:v>
+                  <c:v>2.7000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,7 +699,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$6</c:f>
+              <c:f>工作表1!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -499,9 +732,67 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$2:$F$2</c:f>
+              <c:f>工作表1!$C$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -524,24 +815,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$6:$F$6</c:f>
+              <c:f>工作表1!$C$7:$G$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.17</c:v>
+                  <c:v>2.1700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27</c:v>
+                  <c:v>2.7000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,8 +845,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -573,6 +865,70 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Block Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45926509186351705"/>
+              <c:y val="0.88683438785704316"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -638,7 +994,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Miss</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+                  <a:t> Rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -682,7 +1098,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -771,6 +1187,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>Direct</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+              <a:t> Mapped Cache - Data Cache</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -804,14 +1250,14 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="percentStacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$10</c:f>
+              <c:f>工作表1!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -832,9 +1278,67 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$9:$F$9</c:f>
+              <c:f>工作表1!$C$10:$G$10</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -857,24 +1361,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$10:$F$10</c:f>
+              <c:f>工作表1!$C$11:$G$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.56</c:v>
+                  <c:v>5.5599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.17</c:v>
+                  <c:v>3.1699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.59</c:v>
+                  <c:v>1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -882,7 +1386,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-421E-415A-8982-DB9E98EF8ED0}"/>
+              <c16:uniqueId val="{00000000-0276-473C-9357-D9614FA03FB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -891,7 +1395,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$11</c:f>
+              <c:f>工作表1!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -912,9 +1416,67 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$9:$F$9</c:f>
+              <c:f>工作表1!$C$10:$G$10</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -937,24 +1499,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$11:$F$11</c:f>
+              <c:f>工作表1!$C$12:$G$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.56</c:v>
+                  <c:v>5.5599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.17</c:v>
+                  <c:v>3.1699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.59</c:v>
+                  <c:v>1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,7 +1524,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-421E-415A-8982-DB9E98EF8ED0}"/>
+              <c16:uniqueId val="{00000001-0276-473C-9357-D9614FA03FB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -971,7 +1533,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$12</c:f>
+              <c:f>工作表1!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -992,9 +1554,67 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$9:$F$9</c:f>
+              <c:f>工作表1!$C$10:$G$10</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1017,24 +1637,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$12:$F$12</c:f>
+              <c:f>工作表1!$C$13:$G$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.56</c:v>
+                  <c:v>5.5599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.17</c:v>
+                  <c:v>3.1699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.59</c:v>
+                  <c:v>1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,7 +1662,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-421E-415A-8982-DB9E98EF8ED0}"/>
+              <c16:uniqueId val="{00000002-0276-473C-9357-D9614FA03FB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1051,7 +1671,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>工作表1!$A$13</c:f>
+              <c:f>工作表1!$B$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1072,9 +1692,67 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$B$9:$F$9</c:f>
+              <c:f>工作表1!$C$10:$G$10</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1097,24 +1775,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$13:$F$13</c:f>
+              <c:f>工作表1!$C$14:$G$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.56</c:v>
+                  <c:v>5.5599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.17</c:v>
+                  <c:v>3.1699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.59</c:v>
+                  <c:v>1.5900000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79</c:v>
+                  <c:v>7.9000000000000008E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1122,29 +1800,90 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-421E-415A-8982-DB9E98EF8ED0}"/>
+              <c16:uniqueId val="{00000003-0276-473C-9357-D9614FA03FB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1950836703"/>
-        <c:axId val="1950116015"/>
+        <c:axId val="1061757583"/>
+        <c:axId val="1061070239"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1950836703"/>
+        <c:axId val="1061757583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Block</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1182,7 +1921,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1950116015"/>
+        <c:crossAx val="1061070239"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1190,7 +1929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1950116015"/>
+        <c:axId val="1061070239"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1949,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Miss Rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1241,7 +2036,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1950836703"/>
+        <c:crossAx val="1061757583"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1254,7 +2049,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1285,7 +2080,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2468,22 +3263,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
+      <xdr:colOff>290512</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>3810</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="圖表 2">
+        <xdr:cNvPr id="5" name="圖表 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C937F42-4AC0-4A10-AFBD-3734FCB814EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C0F780E-8D7E-4179-83F0-AD5F03D83F7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2801,216 +3596,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BC19EF-4F6E-4F5B-9D65-01DD79804827}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2.17</v>
-      </c>
-      <c r="C3">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D3">
-        <v>0.54</v>
-      </c>
-      <c r="E3">
-        <v>0.27</v>
-      </c>
-      <c r="F3">
-        <v>0.14000000000000001</v>
+      <c r="C4" s="2">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.09E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>2.17</v>
-      </c>
-      <c r="C4">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D4">
-        <v>0.54</v>
-      </c>
-      <c r="E4">
-        <v>0.27</v>
-      </c>
-      <c r="F4">
-        <v>0.14000000000000001</v>
+      <c r="C5" s="2">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.09E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.4E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>2.17</v>
-      </c>
-      <c r="C5">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D5">
-        <v>0.54</v>
-      </c>
-      <c r="E5">
-        <v>0.27</v>
-      </c>
-      <c r="F5">
-        <v>0.14000000000000001</v>
+      <c r="C6" s="2">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.09E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.4E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>2.17</v>
-      </c>
-      <c r="C6">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D6">
-        <v>0.54</v>
-      </c>
-      <c r="E6">
-        <v>0.27</v>
-      </c>
-      <c r="F6">
-        <v>0.14000000000000001</v>
+      <c r="C7" s="2">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.09E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.4E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10">
-        <v>5.56</v>
-      </c>
-      <c r="C10">
-        <v>3.17</v>
-      </c>
-      <c r="D10">
-        <v>1.59</v>
-      </c>
-      <c r="E10">
-        <v>0.79</v>
-      </c>
-      <c r="F10">
-        <v>0.79</v>
+      <c r="C11" s="2">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>5.56</v>
-      </c>
-      <c r="C11">
-        <v>3.17</v>
-      </c>
-      <c r="D11">
-        <v>1.59</v>
-      </c>
-      <c r="E11">
-        <v>0.79</v>
-      </c>
-      <c r="F11">
-        <v>0.79</v>
+      <c r="C12" s="2">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>5.56</v>
-      </c>
-      <c r="C12">
-        <v>3.17</v>
-      </c>
-      <c r="D12">
-        <v>1.59</v>
-      </c>
-      <c r="E12">
-        <v>0.79</v>
-      </c>
-      <c r="F12">
-        <v>0.79</v>
+      <c r="C13" s="2">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
-        <v>5.56</v>
-      </c>
-      <c r="C13">
-        <v>3.17</v>
-      </c>
-      <c r="D13">
-        <v>1.59</v>
-      </c>
-      <c r="E13">
-        <v>0.79</v>
-      </c>
-      <c r="F13">
-        <v>0.79</v>
+      <c r="C14" s="2">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>7.9000000000000008E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>